<commit_message>
extraccion de islas: algoritmo mas robusto. Densidades obtenidas. Solo falta el calculo del PSD
</commit_message>
<xml_diff>
--- a/pruebas/tiempos-desglosados.xlsx
+++ b/pruebas/tiempos-desglosados.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="47">
   <si>
     <t>Serie</t>
   </si>
@@ -115,12 +115,58 @@
   </si>
   <si>
     <t>45s</t>
+  </si>
+  <si>
+    <t>serie</t>
+  </si>
+  <si>
+    <t>paralela 2 threads</t>
+  </si>
+  <si>
+    <t>optima paralela 2 threads</t>
+  </si>
+  <si>
+    <t>0.0063ms</t>
+  </si>
+  <si>
+    <t>0.0072ms</t>
+  </si>
+  <si>
+    <t>0.0035ms</t>
+  </si>
+  <si>
+    <t>0.0040ms</t>
+  </si>
+  <si>
+    <t>0.0215ms</t>
+  </si>
+  <si>
+    <t>0.0041ms</t>
+  </si>
+  <si>
+    <t>Overhead</t>
+  </si>
+  <si>
+    <t>0.0109ms</t>
+  </si>
+  <si>
+    <t>0.0281ms</t>
+  </si>
+  <si>
+    <t>0.0038ms</t>
+  </si>
+  <si>
+    <t>0.0093ms</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -238,7 +284,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -266,6 +312,21 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -561,17 +622,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:M8"/>
+  <dimension ref="B2:M23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14:L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="4" max="4" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.140625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -757,6 +819,167 @@
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
+    </row>
+    <row r="11" spans="2:13">
+      <c r="F11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13">
+      <c r="D12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="L12" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13">
+      <c r="D13" t="s">
+        <v>34</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="K13" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="L13" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13">
+      <c r="D14" t="s">
+        <v>35</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="I14" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="J14" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="K14" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="L14" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13">
+      <c r="D15" t="s">
+        <v>42</v>
+      </c>
+      <c r="F15" s="14">
+        <v>0</v>
+      </c>
+      <c r="G15" s="14">
+        <v>0.46</v>
+      </c>
+      <c r="H15" s="14">
+        <v>2.0500000000000001E-2</v>
+      </c>
+      <c r="I15" s="14">
+        <v>0.51300000000000001</v>
+      </c>
+      <c r="J15" s="14">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="K15" s="14">
+        <v>0</v>
+      </c>
+      <c r="L15" s="14"/>
+    </row>
+    <row r="20" spans="6:12">
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6"/>
+    </row>
+    <row r="21" spans="6:12">
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="12"/>
+      <c r="K21" s="12"/>
+      <c r="L21" s="12"/>
+    </row>
+    <row r="22" spans="6:12">
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="13"/>
+      <c r="K22" s="13"/>
+      <c r="L22" s="13"/>
+    </row>
+    <row r="23" spans="6:12">
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="11"/>
+      <c r="I23" s="11"/>
+      <c r="J23" s="11"/>
+      <c r="K23" s="11"/>
+      <c r="L23" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>